<commit_message>
journal + diagramme de classe + veille techno
division de l'interface du chrono en 3 fragments
creation du fichier de veille techno
</commit_message>
<xml_diff>
--- a/journal + estimatif.xlsx
+++ b/journal + estimatif.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="21315" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="21315" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plannification" sheetId="1" r:id="rId1"/>
-    <sheet name="Journal" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="actions" sheetId="4" r:id="rId2"/>
+    <sheet name="Journal" sheetId="2" r:id="rId3"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ListeActions" comment="Liste des actions à réaliser">Plannification!$C$5:$C$38</definedName>
+    <definedName name="ListeActions" comment="Liste des actions à réaliser">Plannification!$B$5:$B$38</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="80">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -208,6 +209,73 @@
   </si>
   <si>
     <t>Modification du diagramme de classe suite à migration vers une architecture Fragment</t>
+  </si>
+  <si>
+    <t>Implémentation de la synthese vocale</t>
+  </si>
+  <si>
+    <t>Implémentation du vibreur</t>
+  </si>
+  <si>
+    <t>Modification de la structure des classes métier suite à entretien avec Axel Rinaldi
+Creation d'une classe ChronoModel qui contient les LibExercices, LibSequence et listeSequences et qui permet de faire la sauvegarde et la restoration vers la base de données</t>
+  </si>
+  <si>
+    <t>Android : Classes métier</t>
+  </si>
+  <si>
+    <t>Android : Service</t>
+  </si>
+  <si>
+    <t>Android : Multimédia</t>
+  </si>
+  <si>
+    <t>Android : Synthèse vocale</t>
+  </si>
+  <si>
+    <t>Android : Base de données</t>
+  </si>
+  <si>
+    <t>Android : IHM</t>
+  </si>
+  <si>
+    <t>Windows Phone : Classes métier</t>
+  </si>
+  <si>
+    <t>Windows Phone : Service</t>
+  </si>
+  <si>
+    <t>Windows Phone : Multimédia</t>
+  </si>
+  <si>
+    <t>Windows Phone : Synthèse vocale</t>
+  </si>
+  <si>
+    <t>Windows Phone : Base de données</t>
+  </si>
+  <si>
+    <t>Windows Phone : IHM</t>
+  </si>
+  <si>
+    <t>Ios : Classes métier</t>
+  </si>
+  <si>
+    <t>Ios : Base de données</t>
+  </si>
+  <si>
+    <t>Ios : IHM</t>
+  </si>
+  <si>
+    <t>Réalisation</t>
+  </si>
+  <si>
+    <t>Creation et implémentation des 3 fragments composant la fenetre Chronometre
+gestion des affichages dans les différentes tailles d'écran
+gestion de la rotation de l'écran</t>
+  </si>
+  <si>
+    <t>gestion de la rotation de l'écran pour la persistance du service
+correction du bug du receiver qui n'était pas "unregistered" dans ChronometreActivity</t>
   </si>
 </sst>
 </file>
@@ -302,7 +370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -947,41 +1015,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1277,21 +1315,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1421,8 +1468,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1725,23 +1773,23 @@
   <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B24" sqref="B24:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="45" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="30" width="3.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="29" width="3.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -1749,7 +1797,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11"/>
@@ -1757,118 +1805,119 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
     </row>
     <row r="3" spans="1:31" ht="20.25" customHeight="1"/>
     <row r="4" spans="1:31" ht="72.75" customHeight="1">
       <c r="A4" s="36"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="37" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="38" t="s">
         <v>29</v>
       </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
       <c r="F4" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L4" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M4" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N4" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O4" s="9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P4" s="9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q4" s="9">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R4" s="9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S4" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T4" s="9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U4" s="9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="V4" s="9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="W4" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="X4" s="9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Y4" s="9">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Z4" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AA4" s="9">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB4" s="9">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC4" s="9">
-        <v>24</v>
-      </c>
-      <c r="AD4" s="9">
         <v>25</v>
       </c>
-      <c r="AE4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:31" ht="15.75">
       <c r="A5" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="9">
+      <c r="C5" s="9">
         <v>3</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
@@ -1883,20 +1932,19 @@
       <c r="AA5" s="9"/>
       <c r="AB5" s="9"/>
       <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="34"/>
+      <c r="AD5" s="34"/>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1920,29 +1968,28 @@
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="34"/>
+      <c r="AD6" s="34"/>
     </row>
     <row r="7" spans="1:31">
       <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="9">
+      <c r="C7" s="9">
         <v>4</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
@@ -1957,26 +2004,25 @@
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
       <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="34"/>
+      <c r="AD7" s="34"/>
     </row>
     <row r="8" spans="1:31" ht="15.75">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="9">
+      <c r="C8" s="9">
         <v>5</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
@@ -1996,27 +2042,26 @@
       <c r="AA8" s="9"/>
       <c r="AB8" s="9"/>
       <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="34"/>
+      <c r="AD8" s="34"/>
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="C9" s="9">
         <v>5</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="9"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
@@ -2033,28 +2078,27 @@
       <c r="AA9" s="9"/>
       <c r="AB9" s="9"/>
       <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="34"/>
+      <c r="AD9" s="34"/>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="9">
+      <c r="C10" s="9">
         <v>6</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -2070,24 +2114,23 @@
       <c r="AA10" s="9"/>
       <c r="AB10" s="9"/>
       <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="34"/>
+      <c r="AD10" s="34"/>
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="9">
+      <c r="B11" s="35"/>
+      <c r="C11" s="9">
         <v>6</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -2095,43 +2138,40 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="9"/>
       <c r="X11" s="9"/>
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="34"/>
+      <c r="AD11" s="34"/>
     </row>
     <row r="12" spans="1:31" ht="15.75">
       <c r="A12" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="B12" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -2148,19 +2188,18 @@
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="34"/>
+      <c r="AD12" s="34"/>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="B13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="9">
         <v>1</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -2168,8 +2207,8 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
@@ -2185,19 +2224,18 @@
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="34"/>
+      <c r="AD13" s="34"/>
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="B14" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="9">
         <v>0.5</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -2206,8 +2244,8 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="9"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
@@ -2222,19 +2260,18 @@
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
       <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="34"/>
+      <c r="AD14" s="34"/>
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="B15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="9">
         <v>0.5</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -2243,8 +2280,8 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
@@ -2259,19 +2296,18 @@
       <c r="AA15" s="9"/>
       <c r="AB15" s="9"/>
       <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="34"/>
+      <c r="AD15" s="34"/>
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="B16" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -2281,8 +2317,8 @@
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
@@ -2296,19 +2332,18 @@
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="34"/>
-    </row>
-    <row r="17" spans="1:31">
+      <c r="AD16" s="34"/>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="B17" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -2319,11 +2354,11 @@
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
+      <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="14"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="9"/>
       <c r="U17" s="9"/>
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
@@ -2331,23 +2366,20 @@
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
-      <c r="AB17" s="9"/>
+      <c r="AB17" s="34"/>
       <c r="AC17" s="34"/>
       <c r="AD17" s="34"/>
-      <c r="AE17" s="34"/>
-    </row>
-    <row r="18" spans="1:31">
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" s="34"/>
-      <c r="B18" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="B18" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="9">
         <v>2</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -2360,31 +2392,30 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
+      <c r="T18" s="9"/>
       <c r="U18" s="9"/>
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
+      <c r="AA18" s="34"/>
       <c r="AB18" s="34"/>
       <c r="AC18" s="34"/>
       <c r="AD18" s="34"/>
-      <c r="AE18" s="34"/>
-    </row>
-    <row r="19" spans="1:31">
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="B19" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="9">
         <v>1</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -2399,29 +2430,28 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="9"/>
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
+      <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
       <c r="AC19" s="34"/>
       <c r="AD19" s="34"/>
-      <c r="AE19" s="34"/>
-    </row>
-    <row r="20" spans="1:31">
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="9">
+      <c r="B20" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="9">
         <v>0.5</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -2437,28 +2467,27 @@
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="9"/>
       <c r="W20" s="9"/>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
+      <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
       <c r="AC20" s="34"/>
       <c r="AD20" s="34"/>
-      <c r="AE20" s="34"/>
-    </row>
-    <row r="21" spans="1:31">
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="B21" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="9">
         <v>0.5</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -2474,28 +2503,27 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
+      <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
       <c r="AC21" s="34"/>
       <c r="AD21" s="34"/>
-      <c r="AE21" s="34"/>
-    </row>
-    <row r="22" spans="1:31">
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="B22" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="9">
         <v>1</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -2512,27 +2540,26 @@
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="9"/>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
+      <c r="Z22" s="34"/>
       <c r="AA22" s="34"/>
       <c r="AB22" s="34"/>
       <c r="AC22" s="34"/>
       <c r="AD22" s="34"/>
-      <c r="AE22" s="34"/>
-    </row>
-    <row r="23" spans="1:31">
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="B23" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="9">
         <v>2</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -2550,28 +2577,25 @@
       <c r="T23" s="9"/>
       <c r="U23" s="9"/>
       <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
+      <c r="W23" s="15"/>
       <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
       <c r="AC23" s="34"/>
       <c r="AD23" s="34"/>
-      <c r="AE23" s="34"/>
-    </row>
-    <row r="24" spans="1:31">
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="34"/>
-      <c r="B24" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="9">
+      <c r="B24" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="9">
         <v>1</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -2591,24 +2615,23 @@
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
       <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="9"/>
       <c r="AA24" s="9"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="34"/>
-    </row>
-    <row r="25" spans="1:31">
+      <c r="AD24" s="34"/>
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="9">
+      <c r="B25" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="9">
         <v>1</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -2629,23 +2652,22 @@
       <c r="W25" s="9"/>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="34"/>
-    </row>
-    <row r="26" spans="1:31">
+      <c r="AD25" s="34"/>
+    </row>
+    <row r="26" spans="1:30">
       <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="9">
+      <c r="B26" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -2667,18 +2689,17 @@
       <c r="X26" s="9"/>
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="15"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="34"/>
-    </row>
-    <row r="27" spans="1:31">
+      <c r="AD26" s="34"/>
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -2703,8 +2724,7 @@
       <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="34"/>
+      <c r="AD27" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2714,10 +2734,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" customHeight="1">
+      <c r="A1" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" customHeight="1">
+      <c r="A2" s="35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" customHeight="1">
+      <c r="A3" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" customHeight="1">
+      <c r="A4" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15" customHeight="1">
+      <c r="A5" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15" customHeight="1">
+      <c r="A6" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15" customHeight="1"/>
+    <row r="8" spans="1:1" ht="15" customHeight="1"/>
+    <row r="9" spans="1:1" ht="15" customHeight="1">
+      <c r="A9" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15" customHeight="1">
+      <c r="A10" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15" customHeight="1">
+      <c r="A11" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" customHeight="1">
+      <c r="A12" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15" customHeight="1">
+      <c r="A13" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15" customHeight="1">
+      <c r="A14" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15" customHeight="1"/>
+    <row r="16" spans="1:1" ht="15" customHeight="1"/>
+    <row r="17" spans="1:1" ht="15" customHeight="1"/>
+    <row r="18" spans="1:1" ht="15" customHeight="1">
+      <c r="A18" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" customHeight="1">
+      <c r="A19" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" customHeight="1">
+      <c r="A20" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" customHeight="1"/>
+    <row r="22" spans="1:1" ht="15" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2745,7 +2865,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="125">
+      <c r="A4" s="130">
         <v>42019</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2756,7 +2876,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="126"/>
+      <c r="A5" s="131"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -2765,7 +2885,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="127"/>
+      <c r="A6" s="132"/>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
@@ -2774,7 +2894,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="125">
+      <c r="A7" s="130">
         <v>42039</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2785,7 +2905,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="127"/>
+      <c r="A8" s="132"/>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2794,7 +2914,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="125">
+      <c r="A9" s="130">
         <v>42043</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2805,7 +2925,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="127"/>
+      <c r="A10" s="132"/>
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -2814,7 +2934,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="125">
+      <c r="A11" s="130">
         <v>42046</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2825,7 +2945,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="127"/>
+      <c r="A12" s="132"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
@@ -2834,18 +2954,18 @@
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A13" s="125">
+      <c r="A13" s="130">
         <v>42049</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="127"/>
+      <c r="A14" s="132"/>
       <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
@@ -2854,18 +2974,18 @@
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A15" s="125">
+      <c r="A15" s="130">
         <v>42052</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="127"/>
+      <c r="A16" s="132"/>
       <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
@@ -2874,7 +2994,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" ht="60">
-      <c r="A17" s="125">
+      <c r="A17" s="130">
         <v>42053</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2885,36 +3005,36 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="126"/>
+      <c r="A18" s="131"/>
       <c r="B18" s="5" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A19" s="127"/>
+      <c r="A19" s="132"/>
       <c r="B19" s="7" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A20" s="125">
+      <c r="A20" s="130">
         <v>42058</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="126"/>
+      <c r="A21" s="131"/>
       <c r="B21" s="30" t="s">
         <v>2</v>
       </c>
@@ -2923,16 +3043,16 @@
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="126"/>
+      <c r="A22" s="131"/>
       <c r="B22" s="5" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="127"/>
+      <c r="A23" s="132"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
@@ -2941,27 +3061,27 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1">
-      <c r="A24" s="125">
+      <c r="A24" s="130">
         <v>42059</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A25" s="127"/>
+      <c r="A25" s="132"/>
       <c r="B25" s="7" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="128">
+      <c r="A26" s="127">
         <v>42067</v>
       </c>
       <c r="B26" s="85" t="s">
@@ -2972,7 +3092,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A27" s="129"/>
+      <c r="A27" s="128"/>
       <c r="B27" s="87" t="s">
         <v>25</v>
       </c>
@@ -2992,7 +3112,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="173">
+      <c r="A29" s="127">
         <v>42072</v>
       </c>
       <c r="B29" s="85" t="s">
@@ -3003,27 +3123,27 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="174"/>
+      <c r="A30" s="128"/>
       <c r="B30" s="87" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C30" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="173">
+      <c r="A31" s="127">
         <v>42074</v>
       </c>
       <c r="B31" s="85" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C31" s="86" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A32" s="174"/>
+      <c r="A32" s="128"/>
       <c r="B32" s="87" t="s">
         <v>2</v>
       </c>
@@ -3031,18 +3151,78 @@
         <v>58</v>
       </c>
     </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="127">
+        <v>42075</v>
+      </c>
+      <c r="B33" s="85" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="86" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="129"/>
+      <c r="B34" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="126" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="45">
+      <c r="A35" s="129"/>
+      <c r="B35" s="125" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A36" s="128"/>
+      <c r="B36" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45">
+      <c r="A37" s="32">
+        <v>42076</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="176" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30">
+      <c r="B38" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="176" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tache non référencée" error="La tâche entrée n'est pas référencée dans le planning_x000a_" sqref="B1:B1048576">
@@ -3054,7 +3234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA72"/>
   <sheetViews>
@@ -3080,10 +3260,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickTop="1">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="149"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
@@ -3092,8 +3272,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="150"/>
-      <c r="B3" s="151"/>
+      <c r="A3" s="153"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
@@ -3102,8 +3282,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="150"/>
-      <c r="B4" s="151"/>
+      <c r="A4" s="153"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
@@ -3112,8 +3292,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="150"/>
-      <c r="B5" s="151"/>
+      <c r="A5" s="153"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
@@ -3122,8 +3302,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="150"/>
-      <c r="B6" s="151"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
@@ -3132,8 +3312,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="152"/>
-      <c r="B7" s="153"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
@@ -3142,10 +3322,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="154" t="s">
+      <c r="A8" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="157" t="s">
+      <c r="B8" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3156,8 +3336,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="155"/>
-      <c r="B9" s="158"/>
+      <c r="A9" s="158"/>
+      <c r="B9" s="161"/>
       <c r="C9" s="24" t="s">
         <v>7</v>
       </c>
@@ -3166,8 +3346,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="155"/>
-      <c r="B10" s="158"/>
+      <c r="A10" s="158"/>
+      <c r="B10" s="161"/>
       <c r="C10" s="24" t="s">
         <v>9</v>
       </c>
@@ -3176,8 +3356,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="155"/>
-      <c r="B11" s="158"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="161"/>
       <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
@@ -3186,8 +3366,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="155"/>
-      <c r="B12" s="158"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="161"/>
       <c r="C12" s="24" t="s">
         <v>10</v>
       </c>
@@ -3196,8 +3376,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="156"/>
-      <c r="B13" s="159"/>
+      <c r="A13" s="159"/>
+      <c r="B13" s="162"/>
       <c r="C13" s="26" t="s">
         <v>12</v>
       </c>
@@ -3453,12 +3633,12 @@
     <row r="47" spans="1:4" ht="76.5" customHeight="1" thickBot="1"/>
     <row r="48" spans="1:4" ht="15.75" hidden="1" thickBot="1"/>
     <row r="49" spans="1:27" ht="23.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A49" s="170" t="s">
+      <c r="A49" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="171"/>
-      <c r="C49" s="171"/>
-      <c r="D49" s="172"/>
+      <c r="B49" s="174"/>
+      <c r="C49" s="174"/>
+      <c r="D49" s="175"/>
       <c r="E49" s="120">
         <v>1</v>
       </c>
@@ -3530,10 +3710,10 @@
       </c>
     </row>
     <row r="50" spans="1:27" ht="24.75">
-      <c r="A50" s="160" t="s">
+      <c r="A50" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="161"/>
+      <c r="B50" s="164"/>
       <c r="C50" s="116" t="s">
         <v>46</v>
       </c>
@@ -3565,8 +3745,8 @@
       <c r="AA50" s="119"/>
     </row>
     <row r="51" spans="1:27" ht="36.75">
-      <c r="A51" s="160"/>
-      <c r="B51" s="161"/>
+      <c r="A51" s="163"/>
+      <c r="B51" s="164"/>
       <c r="C51" s="93" t="s">
         <v>26</v>
       </c>
@@ -3598,8 +3778,8 @@
       <c r="AA51" s="92"/>
     </row>
     <row r="52" spans="1:27" ht="36.75">
-      <c r="A52" s="162"/>
-      <c r="B52" s="163"/>
+      <c r="A52" s="165"/>
+      <c r="B52" s="166"/>
       <c r="C52" s="93" t="s">
         <v>25</v>
       </c>
@@ -3631,10 +3811,10 @@
       <c r="AA52" s="92"/>
     </row>
     <row r="53" spans="1:27" ht="24.75">
-      <c r="A53" s="164" t="s">
+      <c r="A53" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="165"/>
+      <c r="B53" s="168"/>
       <c r="C53" s="97" t="s">
         <v>1</v>
       </c>
@@ -3666,8 +3846,8 @@
       <c r="AA53" s="92"/>
     </row>
     <row r="54" spans="1:27" ht="24.75">
-      <c r="A54" s="166"/>
-      <c r="B54" s="167"/>
+      <c r="A54" s="169"/>
+      <c r="B54" s="170"/>
       <c r="C54" s="97" t="s">
         <v>3</v>
       </c>
@@ -3699,8 +3879,8 @@
       <c r="AA54" s="92"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="168"/>
-      <c r="B55" s="169"/>
+      <c r="A55" s="171"/>
+      <c r="B55" s="172"/>
       <c r="C55" s="97" t="s">
         <v>2</v>
       </c>
@@ -3765,10 +3945,10 @@
       <c r="AA56" s="92"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A57" s="130" t="s">
+      <c r="A57" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="131"/>
+      <c r="B57" s="134"/>
       <c r="C57" s="104" t="s">
         <v>8</v>
       </c>
@@ -3800,8 +3980,8 @@
       <c r="AA57" s="92"/>
     </row>
     <row r="58" spans="1:27" ht="15" customHeight="1">
-      <c r="A58" s="132"/>
-      <c r="B58" s="133"/>
+      <c r="A58" s="135"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="104" t="s">
         <v>7</v>
       </c>
@@ -3833,8 +4013,8 @@
       <c r="AA58" s="92"/>
     </row>
     <row r="59" spans="1:27" ht="15" customHeight="1">
-      <c r="A59" s="132"/>
-      <c r="B59" s="133"/>
+      <c r="A59" s="135"/>
+      <c r="B59" s="136"/>
       <c r="C59" s="104" t="s">
         <v>48</v>
       </c>
@@ -3866,8 +4046,8 @@
       <c r="AA59" s="92"/>
     </row>
     <row r="60" spans="1:27" ht="15" customHeight="1">
-      <c r="A60" s="132"/>
-      <c r="B60" s="133"/>
+      <c r="A60" s="135"/>
+      <c r="B60" s="136"/>
       <c r="C60" s="104" t="s">
         <v>49</v>
       </c>
@@ -3899,8 +4079,8 @@
       <c r="AA60" s="92"/>
     </row>
     <row r="61" spans="1:27" ht="15" customHeight="1">
-      <c r="A61" s="132"/>
-      <c r="B61" s="133"/>
+      <c r="A61" s="135"/>
+      <c r="B61" s="136"/>
       <c r="C61" s="104" t="s">
         <v>54</v>
       </c>
@@ -3932,8 +4112,8 @@
       <c r="AA61" s="92"/>
     </row>
     <row r="62" spans="1:27" ht="15" customHeight="1">
-      <c r="A62" s="134"/>
-      <c r="B62" s="135"/>
+      <c r="A62" s="137"/>
+      <c r="B62" s="138"/>
       <c r="C62" s="104" t="s">
         <v>12</v>
       </c>
@@ -3965,10 +4145,10 @@
       <c r="AA62" s="92"/>
     </row>
     <row r="63" spans="1:27" ht="15" customHeight="1">
-      <c r="A63" s="136" t="s">
+      <c r="A63" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="137"/>
+      <c r="B63" s="140"/>
       <c r="C63" s="106" t="s">
         <v>8</v>
       </c>
@@ -4000,8 +4180,8 @@
       <c r="AA63" s="108"/>
     </row>
     <row r="64" spans="1:27" ht="15" customHeight="1">
-      <c r="A64" s="138"/>
-      <c r="B64" s="139"/>
+      <c r="A64" s="141"/>
+      <c r="B64" s="142"/>
       <c r="C64" s="106" t="s">
         <v>7</v>
       </c>
@@ -4033,8 +4213,8 @@
       <c r="AA64" s="108"/>
     </row>
     <row r="65" spans="1:27" ht="15" customHeight="1">
-      <c r="A65" s="138"/>
-      <c r="B65" s="139"/>
+      <c r="A65" s="141"/>
+      <c r="B65" s="142"/>
       <c r="C65" s="106" t="s">
         <v>48</v>
       </c>
@@ -4066,8 +4246,8 @@
       <c r="AA65" s="108"/>
     </row>
     <row r="66" spans="1:27" ht="15" customHeight="1">
-      <c r="A66" s="138"/>
-      <c r="B66" s="139"/>
+      <c r="A66" s="141"/>
+      <c r="B66" s="142"/>
       <c r="C66" s="106" t="s">
         <v>49</v>
       </c>
@@ -4099,8 +4279,8 @@
       <c r="AA66" s="108"/>
     </row>
     <row r="67" spans="1:27" ht="15" customHeight="1">
-      <c r="A67" s="138"/>
-      <c r="B67" s="139"/>
+      <c r="A67" s="141"/>
+      <c r="B67" s="142"/>
       <c r="C67" s="106" t="s">
         <v>54</v>
       </c>
@@ -4132,8 +4312,8 @@
       <c r="AA67" s="108"/>
     </row>
     <row r="68" spans="1:27" ht="15" customHeight="1">
-      <c r="A68" s="140"/>
-      <c r="B68" s="141"/>
+      <c r="A68" s="143"/>
+      <c r="B68" s="144"/>
       <c r="C68" s="106" t="s">
         <v>12</v>
       </c>
@@ -4165,10 +4345,10 @@
       <c r="AA68" s="108"/>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1">
-      <c r="A69" s="142" t="s">
+      <c r="A69" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="143"/>
+      <c r="B69" s="146"/>
       <c r="C69" s="110" t="s">
         <v>8</v>
       </c>
@@ -4200,8 +4380,8 @@
       <c r="AA69" s="92"/>
     </row>
     <row r="70" spans="1:27" ht="15" customHeight="1">
-      <c r="A70" s="144"/>
-      <c r="B70" s="145"/>
+      <c r="A70" s="147"/>
+      <c r="B70" s="148"/>
       <c r="C70" s="110" t="s">
         <v>54</v>
       </c>
@@ -4233,8 +4413,8 @@
       <c r="AA70" s="92"/>
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A71" s="146"/>
-      <c r="B71" s="147"/>
+      <c r="A71" s="149"/>
+      <c r="B71" s="150"/>
       <c r="C71" s="112" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
journal + regle de nommage + bug
</commit_message>
<xml_diff>
--- a/journal + estimatif.xlsx
+++ b/journal + estimatif.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="86">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -276,6 +276,33 @@
   <si>
     <t>gestion de la rotation de l'écran pour la persistance du service
 correction du bug du receiver qui n'était pas "unregistered" dans ChronometreActivity</t>
+  </si>
+  <si>
+    <t>Detection d'un bug obligeant d'utiliser la derniere version des librairies</t>
+  </si>
+  <si>
+    <t>Creation de la classe ListeSequencesActivity + Frag_ListeSeq_BtnRetour + Frag_ListeSeq_BtnAjoutSeq
+creation des dialog repetition, durée et confirmation suppression
+correction de l'erreur "liste sequence vide"</t>
+  </si>
+  <si>
+    <t>Creation d'un unique Callback pour les boutons
+ListeSequencesActivity : gestion du click long sur les items
+Creation de AjoutSequenceActivity 
+Creation de AjoutExerciceActivity
+Creation de EditionSequenceActivity
+Creation de Frag_Dialog_EnregistrementSeq
+gestion dépassement du temps listeSequences
+corrections de bug + optimisation du code</t>
+  </si>
+  <si>
+    <t>implémentation fonction egale et getClone dans les classes métier</t>
+  </si>
+  <si>
+    <t>mise à jour diagramme de classe</t>
+  </si>
+  <si>
+    <t>regle de nommage android</t>
   </si>
 </sst>
 </file>
@@ -285,7 +312,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-yy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +333,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1016,10 +1050,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1321,6 +1359,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1468,11 +1512,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2834,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2865,7 +2907,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="130">
+      <c r="A4" s="132">
         <v>42019</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2876,7 +2918,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="131"/>
+      <c r="A5" s="133"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -2885,7 +2927,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="132"/>
+      <c r="A6" s="134"/>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
@@ -2894,7 +2936,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="130">
+      <c r="A7" s="132">
         <v>42039</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2905,7 +2947,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="132"/>
+      <c r="A8" s="134"/>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -2914,7 +2956,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="130">
+      <c r="A9" s="132">
         <v>42043</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2925,7 +2967,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="132"/>
+      <c r="A10" s="134"/>
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -2934,7 +2976,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="130">
+      <c r="A11" s="132">
         <v>42046</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2945,7 +2987,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="132"/>
+      <c r="A12" s="134"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
@@ -2954,7 +2996,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A13" s="130">
+      <c r="A13" s="132">
         <v>42049</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2965,7 +3007,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="132"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
@@ -2974,7 +3016,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A15" s="130">
+      <c r="A15" s="132">
         <v>42052</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2985,7 +3027,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="132"/>
+      <c r="A16" s="134"/>
       <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
@@ -2994,7 +3036,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" ht="60">
-      <c r="A17" s="130">
+      <c r="A17" s="132">
         <v>42053</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -3005,7 +3047,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="131"/>
+      <c r="A18" s="133"/>
       <c r="B18" s="5" t="s">
         <v>62</v>
       </c>
@@ -3014,7 +3056,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A19" s="132"/>
+      <c r="A19" s="134"/>
       <c r="B19" s="7" t="s">
         <v>66</v>
       </c>
@@ -3023,7 +3065,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A20" s="130">
+      <c r="A20" s="132">
         <v>42058</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -3034,7 +3076,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="131"/>
+      <c r="A21" s="133"/>
       <c r="B21" s="30" t="s">
         <v>2</v>
       </c>
@@ -3043,7 +3085,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="131"/>
+      <c r="A22" s="133"/>
       <c r="B22" s="5" t="s">
         <v>67</v>
       </c>
@@ -3052,7 +3094,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="132"/>
+      <c r="A23" s="134"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
@@ -3061,7 +3103,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1">
-      <c r="A24" s="130">
+      <c r="A24" s="132">
         <v>42059</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3072,7 +3114,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A25" s="132"/>
+      <c r="A25" s="134"/>
       <c r="B25" s="7" t="s">
         <v>63</v>
       </c>
@@ -3081,7 +3123,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="127">
+      <c r="A26" s="129">
         <v>42067</v>
       </c>
       <c r="B26" s="85" t="s">
@@ -3092,7 +3134,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A27" s="128"/>
+      <c r="A27" s="130"/>
       <c r="B27" s="87" t="s">
         <v>25</v>
       </c>
@@ -3112,7 +3154,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="127">
+      <c r="A29" s="129">
         <v>42072</v>
       </c>
       <c r="B29" s="85" t="s">
@@ -3123,7 +3165,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="128"/>
+      <c r="A30" s="130"/>
       <c r="B30" s="87" t="s">
         <v>67</v>
       </c>
@@ -3132,7 +3174,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="127">
+      <c r="A31" s="129">
         <v>42074</v>
       </c>
       <c r="B31" s="85" t="s">
@@ -3143,7 +3185,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A32" s="128"/>
+      <c r="A32" s="130"/>
       <c r="B32" s="87" t="s">
         <v>2</v>
       </c>
@@ -3152,7 +3194,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="127">
+      <c r="A33" s="129">
         <v>42075</v>
       </c>
       <c r="B33" s="85" t="s">
@@ -3163,7 +3205,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="129"/>
+      <c r="A34" s="131"/>
       <c r="B34" s="125" t="s">
         <v>64</v>
       </c>
@@ -3172,7 +3214,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="45">
-      <c r="A35" s="129"/>
+      <c r="A35" s="131"/>
       <c r="B35" s="125" t="s">
         <v>62</v>
       </c>
@@ -3181,7 +3223,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A36" s="128"/>
+      <c r="A36" s="130"/>
       <c r="B36" s="87" t="s">
         <v>2</v>
       </c>
@@ -3196,7 +3238,7 @@
       <c r="B37" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="176" t="s">
+      <c r="C37" s="127" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3204,8 +3246,62 @@
       <c r="B38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="176" t="s">
+      <c r="C38" s="127" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="32">
+        <v>42077</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="128" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="60">
+      <c r="B40" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="127" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="120">
+      <c r="A41" s="32">
+        <v>42078</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="127" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3229,8 +3325,11 @@
       <formula1>ListeActions</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C39" r:id="rId1" display="Detection d'un bug encore non corrigé par google : bug"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3260,10 +3359,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickTop="1">
-      <c r="A2" s="151" t="s">
+      <c r="A2" s="153" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="152"/>
+      <c r="B2" s="154"/>
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
@@ -3272,8 +3371,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="153"/>
-      <c r="B3" s="154"/>
+      <c r="A3" s="155"/>
+      <c r="B3" s="156"/>
       <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
@@ -3282,8 +3381,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="153"/>
-      <c r="B4" s="154"/>
+      <c r="A4" s="155"/>
+      <c r="B4" s="156"/>
       <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
@@ -3292,8 +3391,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="153"/>
-      <c r="B5" s="154"/>
+      <c r="A5" s="155"/>
+      <c r="B5" s="156"/>
       <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
@@ -3302,8 +3401,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="153"/>
-      <c r="B6" s="154"/>
+      <c r="A6" s="155"/>
+      <c r="B6" s="156"/>
       <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
@@ -3312,8 +3411,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="155"/>
-      <c r="B7" s="156"/>
+      <c r="A7" s="157"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
@@ -3322,10 +3421,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="157" t="s">
+      <c r="A8" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="162" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3336,8 +3435,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="158"/>
-      <c r="B9" s="161"/>
+      <c r="A9" s="160"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="24" t="s">
         <v>7</v>
       </c>
@@ -3346,8 +3445,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="158"/>
-      <c r="B10" s="161"/>
+      <c r="A10" s="160"/>
+      <c r="B10" s="163"/>
       <c r="C10" s="24" t="s">
         <v>9</v>
       </c>
@@ -3356,8 +3455,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="158"/>
-      <c r="B11" s="161"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="163"/>
       <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
@@ -3366,8 +3465,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="158"/>
-      <c r="B12" s="161"/>
+      <c r="A12" s="160"/>
+      <c r="B12" s="163"/>
       <c r="C12" s="24" t="s">
         <v>10</v>
       </c>
@@ -3376,8 +3475,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="159"/>
-      <c r="B13" s="162"/>
+      <c r="A13" s="161"/>
+      <c r="B13" s="164"/>
       <c r="C13" s="26" t="s">
         <v>12</v>
       </c>
@@ -3633,12 +3732,12 @@
     <row r="47" spans="1:4" ht="76.5" customHeight="1" thickBot="1"/>
     <row r="48" spans="1:4" ht="15.75" hidden="1" thickBot="1"/>
     <row r="49" spans="1:27" ht="23.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A49" s="173" t="s">
+      <c r="A49" s="175" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="174"/>
-      <c r="C49" s="174"/>
-      <c r="D49" s="175"/>
+      <c r="B49" s="176"/>
+      <c r="C49" s="176"/>
+      <c r="D49" s="177"/>
       <c r="E49" s="120">
         <v>1</v>
       </c>
@@ -3710,10 +3809,10 @@
       </c>
     </row>
     <row r="50" spans="1:27" ht="24.75">
-      <c r="A50" s="163" t="s">
+      <c r="A50" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="164"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="116" t="s">
         <v>46</v>
       </c>
@@ -3745,8 +3844,8 @@
       <c r="AA50" s="119"/>
     </row>
     <row r="51" spans="1:27" ht="36.75">
-      <c r="A51" s="163"/>
-      <c r="B51" s="164"/>
+      <c r="A51" s="165"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="93" t="s">
         <v>26</v>
       </c>
@@ -3778,8 +3877,8 @@
       <c r="AA51" s="92"/>
     </row>
     <row r="52" spans="1:27" ht="36.75">
-      <c r="A52" s="165"/>
-      <c r="B52" s="166"/>
+      <c r="A52" s="167"/>
+      <c r="B52" s="168"/>
       <c r="C52" s="93" t="s">
         <v>25</v>
       </c>
@@ -3811,10 +3910,10 @@
       <c r="AA52" s="92"/>
     </row>
     <row r="53" spans="1:27" ht="24.75">
-      <c r="A53" s="167" t="s">
+      <c r="A53" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="168"/>
+      <c r="B53" s="170"/>
       <c r="C53" s="97" t="s">
         <v>1</v>
       </c>
@@ -3846,8 +3945,8 @@
       <c r="AA53" s="92"/>
     </row>
     <row r="54" spans="1:27" ht="24.75">
-      <c r="A54" s="169"/>
-      <c r="B54" s="170"/>
+      <c r="A54" s="171"/>
+      <c r="B54" s="172"/>
       <c r="C54" s="97" t="s">
         <v>3</v>
       </c>
@@ -3879,8 +3978,8 @@
       <c r="AA54" s="92"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="171"/>
-      <c r="B55" s="172"/>
+      <c r="A55" s="173"/>
+      <c r="B55" s="174"/>
       <c r="C55" s="97" t="s">
         <v>2</v>
       </c>
@@ -3945,10 +4044,10 @@
       <c r="AA56" s="92"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A57" s="133" t="s">
+      <c r="A57" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="134"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="104" t="s">
         <v>8</v>
       </c>
@@ -3980,8 +4079,8 @@
       <c r="AA57" s="92"/>
     </row>
     <row r="58" spans="1:27" ht="15" customHeight="1">
-      <c r="A58" s="135"/>
-      <c r="B58" s="136"/>
+      <c r="A58" s="137"/>
+      <c r="B58" s="138"/>
       <c r="C58" s="104" t="s">
         <v>7</v>
       </c>
@@ -4013,8 +4112,8 @@
       <c r="AA58" s="92"/>
     </row>
     <row r="59" spans="1:27" ht="15" customHeight="1">
-      <c r="A59" s="135"/>
-      <c r="B59" s="136"/>
+      <c r="A59" s="137"/>
+      <c r="B59" s="138"/>
       <c r="C59" s="104" t="s">
         <v>48</v>
       </c>
@@ -4046,8 +4145,8 @@
       <c r="AA59" s="92"/>
     </row>
     <row r="60" spans="1:27" ht="15" customHeight="1">
-      <c r="A60" s="135"/>
-      <c r="B60" s="136"/>
+      <c r="A60" s="137"/>
+      <c r="B60" s="138"/>
       <c r="C60" s="104" t="s">
         <v>49</v>
       </c>
@@ -4079,8 +4178,8 @@
       <c r="AA60" s="92"/>
     </row>
     <row r="61" spans="1:27" ht="15" customHeight="1">
-      <c r="A61" s="135"/>
-      <c r="B61" s="136"/>
+      <c r="A61" s="137"/>
+      <c r="B61" s="138"/>
       <c r="C61" s="104" t="s">
         <v>54</v>
       </c>
@@ -4112,8 +4211,8 @@
       <c r="AA61" s="92"/>
     </row>
     <row r="62" spans="1:27" ht="15" customHeight="1">
-      <c r="A62" s="137"/>
-      <c r="B62" s="138"/>
+      <c r="A62" s="139"/>
+      <c r="B62" s="140"/>
       <c r="C62" s="104" t="s">
         <v>12</v>
       </c>
@@ -4145,10 +4244,10 @@
       <c r="AA62" s="92"/>
     </row>
     <row r="63" spans="1:27" ht="15" customHeight="1">
-      <c r="A63" s="139" t="s">
+      <c r="A63" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="140"/>
+      <c r="B63" s="142"/>
       <c r="C63" s="106" t="s">
         <v>8</v>
       </c>
@@ -4180,8 +4279,8 @@
       <c r="AA63" s="108"/>
     </row>
     <row r="64" spans="1:27" ht="15" customHeight="1">
-      <c r="A64" s="141"/>
-      <c r="B64" s="142"/>
+      <c r="A64" s="143"/>
+      <c r="B64" s="144"/>
       <c r="C64" s="106" t="s">
         <v>7</v>
       </c>
@@ -4213,8 +4312,8 @@
       <c r="AA64" s="108"/>
     </row>
     <row r="65" spans="1:27" ht="15" customHeight="1">
-      <c r="A65" s="141"/>
-      <c r="B65" s="142"/>
+      <c r="A65" s="143"/>
+      <c r="B65" s="144"/>
       <c r="C65" s="106" t="s">
         <v>48</v>
       </c>
@@ -4246,8 +4345,8 @@
       <c r="AA65" s="108"/>
     </row>
     <row r="66" spans="1:27" ht="15" customHeight="1">
-      <c r="A66" s="141"/>
-      <c r="B66" s="142"/>
+      <c r="A66" s="143"/>
+      <c r="B66" s="144"/>
       <c r="C66" s="106" t="s">
         <v>49</v>
       </c>
@@ -4279,8 +4378,8 @@
       <c r="AA66" s="108"/>
     </row>
     <row r="67" spans="1:27" ht="15" customHeight="1">
-      <c r="A67" s="141"/>
-      <c r="B67" s="142"/>
+      <c r="A67" s="143"/>
+      <c r="B67" s="144"/>
       <c r="C67" s="106" t="s">
         <v>54</v>
       </c>
@@ -4312,8 +4411,8 @@
       <c r="AA67" s="108"/>
     </row>
     <row r="68" spans="1:27" ht="15" customHeight="1">
-      <c r="A68" s="143"/>
-      <c r="B68" s="144"/>
+      <c r="A68" s="145"/>
+      <c r="B68" s="146"/>
       <c r="C68" s="106" t="s">
         <v>12</v>
       </c>
@@ -4345,10 +4444,10 @@
       <c r="AA68" s="108"/>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1">
-      <c r="A69" s="145" t="s">
+      <c r="A69" s="147" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="146"/>
+      <c r="B69" s="148"/>
       <c r="C69" s="110" t="s">
         <v>8</v>
       </c>
@@ -4380,8 +4479,8 @@
       <c r="AA69" s="92"/>
     </row>
     <row r="70" spans="1:27" ht="15" customHeight="1">
-      <c r="A70" s="147"/>
-      <c r="B70" s="148"/>
+      <c r="A70" s="149"/>
+      <c r="B70" s="150"/>
       <c r="C70" s="110" t="s">
         <v>54</v>
       </c>
@@ -4413,8 +4512,8 @@
       <c r="AA70" s="92"/>
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A71" s="149"/>
-      <c r="B71" s="150"/>
+      <c r="A71" s="151"/>
+      <c r="B71" s="152"/>
       <c r="C71" s="112" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
journal + diagramme de classe
</commit_message>
<xml_diff>
--- a/journal + estimatif.xlsx
+++ b/journal + estimatif.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="93">
   <si>
     <t>Liste des tâches</t>
   </si>
@@ -303,6 +303,30 @@
   </si>
   <si>
     <t>regle de nommage android</t>
+  </si>
+  <si>
+    <t>travail sur la fenetre edition exercice ( tentative de tab fragment mais retour sur une vue normale)</t>
+  </si>
+  <si>
+    <t>creation fenetre editionexerciceplaylist
+remplacement du bouton suppr des items de la listitem par une image
+imlpementation de la fenetre ajoutExercice</t>
+  </si>
+  <si>
+    <t>Remplacement du tableau listSequence par un tableau d'index pointant vers libSequence</t>
+  </si>
+  <si>
+    <t>Ajout d'un tableau stockant les morceaux utilisés dans l'application
+Ajout d'un id aux classes Exercice,ElementSequence, Morceau et Sequence</t>
+  </si>
+  <si>
+    <t>Mise à jour de la base de donnée directement après une modification</t>
+  </si>
+  <si>
+    <t>Lecture des fichiers son de notification</t>
+  </si>
+  <si>
+    <t>Temps (h)</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1081,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1359,12 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1511,6 +1529,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2876,10 +2906,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2889,13 +2919,13 @@
     <col min="3" max="3" width="89.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="33" t="s">
         <v>14</v>
       </c>
@@ -2905,9 +2935,12 @@
       <c r="C3" s="29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1">
-      <c r="A4" s="132">
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="130">
         <v>42019</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2916,27 +2949,36 @@
       <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="133"/>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="131"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A6" s="134"/>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A6" s="132"/>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="132">
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1">
+      <c r="A7" s="130">
         <v>42039</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2945,18 +2987,24 @@
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A8" s="134"/>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A8" s="132"/>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="132">
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1">
+      <c r="A9" s="130">
         <v>42043</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2965,18 +3013,24 @@
       <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A10" s="134"/>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A10" s="132"/>
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="132">
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="130">
         <v>42046</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2985,18 +3039,24 @@
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A12" s="134"/>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A12" s="132"/>
       <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A13" s="132">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="30">
+      <c r="A13" s="130">
         <v>42049</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -3005,18 +3065,24 @@
       <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A14" s="134"/>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A14" s="132"/>
       <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A15" s="132">
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" ht="30">
+      <c r="A15" s="130">
         <v>42052</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -3025,18 +3091,24 @@
       <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="134"/>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A16" s="132"/>
       <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" ht="60">
-      <c r="A17" s="132">
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="60">
+      <c r="A17" s="130">
         <v>42053</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -3045,27 +3117,36 @@
       <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1">
-      <c r="A18" s="133"/>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1">
+      <c r="A18" s="131"/>
       <c r="B18" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A19" s="134"/>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="45.75" thickBot="1">
+      <c r="A19" s="132"/>
       <c r="B19" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" ht="30">
-      <c r="A20" s="132">
+      <c r="D19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="30">
+      <c r="A20" s="130">
         <v>42058</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -3075,8 +3156,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="133"/>
+    <row r="21" spans="1:4" s="1" customFormat="1">
+      <c r="A21" s="131"/>
       <c r="B21" s="30" t="s">
         <v>2</v>
       </c>
@@ -3084,8 +3165,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="133"/>
+    <row r="22" spans="1:4" s="1" customFormat="1">
+      <c r="A22" s="131"/>
       <c r="B22" s="5" t="s">
         <v>67</v>
       </c>
@@ -3093,8 +3174,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="134"/>
+    <row r="23" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A23" s="132"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
@@ -3102,8 +3183,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="1" customFormat="1">
-      <c r="A24" s="132">
+    <row r="24" spans="1:4" s="1" customFormat="1">
+      <c r="A24" s="130">
         <v>42059</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3113,8 +3194,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A25" s="134"/>
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A25" s="132"/>
       <c r="B25" s="7" t="s">
         <v>63</v>
       </c>
@@ -3122,8 +3203,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="129">
+    <row r="26" spans="1:4">
+      <c r="A26" s="127">
         <v>42067</v>
       </c>
       <c r="B26" s="85" t="s">
@@ -3133,8 +3214,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A27" s="130"/>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A27" s="128"/>
       <c r="B27" s="87" t="s">
         <v>25</v>
       </c>
@@ -3142,7 +3223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1">
       <c r="A28" s="122">
         <v>42069</v>
       </c>
@@ -3153,8 +3234,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="129">
+    <row r="29" spans="1:4">
+      <c r="A29" s="127">
         <v>42072</v>
       </c>
       <c r="B29" s="85" t="s">
@@ -3164,8 +3245,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="130"/>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A30" s="128"/>
       <c r="B30" s="87" t="s">
         <v>67</v>
       </c>
@@ -3173,8 +3254,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="129">
+    <row r="31" spans="1:4">
+      <c r="A31" s="127">
         <v>42074</v>
       </c>
       <c r="B31" s="85" t="s">
@@ -3184,8 +3265,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A32" s="130"/>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A32" s="128"/>
       <c r="B32" s="87" t="s">
         <v>2</v>
       </c>
@@ -3193,8 +3274,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="129">
+    <row r="33" spans="1:4">
+      <c r="A33" s="127">
         <v>42075</v>
       </c>
       <c r="B33" s="85" t="s">
@@ -3204,8 +3285,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="131"/>
+    <row r="34" spans="1:4">
+      <c r="A34" s="129"/>
       <c r="B34" s="125" t="s">
         <v>64</v>
       </c>
@@ -3213,8 +3294,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="45">
-      <c r="A35" s="131"/>
+    <row r="35" spans="1:4" ht="45">
+      <c r="A35" s="129"/>
       <c r="B35" s="125" t="s">
         <v>62</v>
       </c>
@@ -3222,8 +3303,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A36" s="130"/>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A36" s="128"/>
       <c r="B36" s="87" t="s">
         <v>2</v>
       </c>
@@ -3231,81 +3312,170 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="45">
-      <c r="A37" s="32">
+    <row r="37" spans="1:4" ht="45">
+      <c r="A37" s="127">
         <v>42076</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="127" t="s">
+      <c r="C37" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
-      <c r="B38" s="9" t="s">
+    <row r="38" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A38" s="128"/>
+      <c r="B38" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="127" t="s">
+      <c r="C38" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="32">
+    <row r="39" spans="1:4">
+      <c r="A39" s="127">
         <v>42077</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="128" t="s">
+      <c r="C39" s="177" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="60">
-      <c r="B40" s="9" t="s">
+    <row r="40" spans="1:4" ht="60.75" thickBot="1">
+      <c r="A40" s="128"/>
+      <c r="B40" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="127" t="s">
+      <c r="C40" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="120">
-      <c r="A41" s="32">
+    <row r="41" spans="1:4" ht="120">
+      <c r="A41" s="127">
         <v>42078</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="127" t="s">
+      <c r="C41" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="B42" s="9" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" s="129"/>
+      <c r="B42" s="125" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="126" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="9" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="129"/>
+      <c r="B43" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="126" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="B44" s="9" t="s">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A44" s="128"/>
+      <c r="B44" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="88" t="s">
         <v>85</v>
       </c>
     </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A45" s="178">
+        <v>42095</v>
+      </c>
+      <c r="B45" s="123" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="124" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45.75" thickBot="1">
+      <c r="A46" s="178">
+        <v>42096</v>
+      </c>
+      <c r="B46" s="123" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="179" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A47" s="178">
+        <v>42097</v>
+      </c>
+      <c r="B47" s="123" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="124" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30">
+      <c r="A48" s="129">
+        <v>42098</v>
+      </c>
+      <c r="B48" s="176" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="129"/>
+      <c r="B49" s="125" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="126" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A50" s="128"/>
+      <c r="B50" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -3359,10 +3529,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30.75" thickTop="1">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="154"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
@@ -3371,8 +3541,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
-      <c r="A3" s="155"/>
-      <c r="B3" s="156"/>
+      <c r="A3" s="153"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
@@ -3381,8 +3551,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="155"/>
-      <c r="B4" s="156"/>
+      <c r="A4" s="153"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
@@ -3391,8 +3561,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
-      <c r="A5" s="155"/>
-      <c r="B5" s="156"/>
+      <c r="A5" s="153"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="22" t="s">
         <v>26</v>
       </c>
@@ -3401,8 +3571,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="155"/>
-      <c r="B6" s="156"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
@@ -3411,8 +3581,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="157"/>
-      <c r="B7" s="158"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
@@ -3421,10 +3591,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="157" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="162" t="s">
+      <c r="B8" s="160" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -3435,8 +3605,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="160"/>
-      <c r="B9" s="163"/>
+      <c r="A9" s="158"/>
+      <c r="B9" s="161"/>
       <c r="C9" s="24" t="s">
         <v>7</v>
       </c>
@@ -3445,8 +3615,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="160"/>
-      <c r="B10" s="163"/>
+      <c r="A10" s="158"/>
+      <c r="B10" s="161"/>
       <c r="C10" s="24" t="s">
         <v>9</v>
       </c>
@@ -3455,8 +3625,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="160"/>
-      <c r="B11" s="163"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="161"/>
       <c r="C11" s="24" t="s">
         <v>11</v>
       </c>
@@ -3465,8 +3635,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="160"/>
-      <c r="B12" s="163"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="161"/>
       <c r="C12" s="24" t="s">
         <v>10</v>
       </c>
@@ -3475,8 +3645,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A13" s="161"/>
-      <c r="B13" s="164"/>
+      <c r="A13" s="159"/>
+      <c r="B13" s="162"/>
       <c r="C13" s="26" t="s">
         <v>12</v>
       </c>
@@ -3732,12 +3902,12 @@
     <row r="47" spans="1:4" ht="76.5" customHeight="1" thickBot="1"/>
     <row r="48" spans="1:4" ht="15.75" hidden="1" thickBot="1"/>
     <row r="49" spans="1:27" ht="23.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A49" s="175" t="s">
+      <c r="A49" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="176"/>
-      <c r="C49" s="176"/>
-      <c r="D49" s="177"/>
+      <c r="B49" s="174"/>
+      <c r="C49" s="174"/>
+      <c r="D49" s="175"/>
       <c r="E49" s="120">
         <v>1</v>
       </c>
@@ -3809,10 +3979,10 @@
       </c>
     </row>
     <row r="50" spans="1:27" ht="24.75">
-      <c r="A50" s="165" t="s">
+      <c r="A50" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="166"/>
+      <c r="B50" s="164"/>
       <c r="C50" s="116" t="s">
         <v>46</v>
       </c>
@@ -3844,8 +4014,8 @@
       <c r="AA50" s="119"/>
     </row>
     <row r="51" spans="1:27" ht="36.75">
-      <c r="A51" s="165"/>
-      <c r="B51" s="166"/>
+      <c r="A51" s="163"/>
+      <c r="B51" s="164"/>
       <c r="C51" s="93" t="s">
         <v>26</v>
       </c>
@@ -3877,8 +4047,8 @@
       <c r="AA51" s="92"/>
     </row>
     <row r="52" spans="1:27" ht="36.75">
-      <c r="A52" s="167"/>
-      <c r="B52" s="168"/>
+      <c r="A52" s="165"/>
+      <c r="B52" s="166"/>
       <c r="C52" s="93" t="s">
         <v>25</v>
       </c>
@@ -3910,10 +4080,10 @@
       <c r="AA52" s="92"/>
     </row>
     <row r="53" spans="1:27" ht="24.75">
-      <c r="A53" s="169" t="s">
+      <c r="A53" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="170"/>
+      <c r="B53" s="168"/>
       <c r="C53" s="97" t="s">
         <v>1</v>
       </c>
@@ -3945,8 +4115,8 @@
       <c r="AA53" s="92"/>
     </row>
     <row r="54" spans="1:27" ht="24.75">
-      <c r="A54" s="171"/>
-      <c r="B54" s="172"/>
+      <c r="A54" s="169"/>
+      <c r="B54" s="170"/>
       <c r="C54" s="97" t="s">
         <v>3</v>
       </c>
@@ -3978,8 +4148,8 @@
       <c r="AA54" s="92"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="173"/>
-      <c r="B55" s="174"/>
+      <c r="A55" s="171"/>
+      <c r="B55" s="172"/>
       <c r="C55" s="97" t="s">
         <v>2</v>
       </c>
@@ -4044,10 +4214,10 @@
       <c r="AA56" s="92"/>
     </row>
     <row r="57" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="134"/>
       <c r="C57" s="104" t="s">
         <v>8</v>
       </c>
@@ -4079,8 +4249,8 @@
       <c r="AA57" s="92"/>
     </row>
     <row r="58" spans="1:27" ht="15" customHeight="1">
-      <c r="A58" s="137"/>
-      <c r="B58" s="138"/>
+      <c r="A58" s="135"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="104" t="s">
         <v>7</v>
       </c>
@@ -4112,8 +4282,8 @@
       <c r="AA58" s="92"/>
     </row>
     <row r="59" spans="1:27" ht="15" customHeight="1">
-      <c r="A59" s="137"/>
-      <c r="B59" s="138"/>
+      <c r="A59" s="135"/>
+      <c r="B59" s="136"/>
       <c r="C59" s="104" t="s">
         <v>48</v>
       </c>
@@ -4145,8 +4315,8 @@
       <c r="AA59" s="92"/>
     </row>
     <row r="60" spans="1:27" ht="15" customHeight="1">
-      <c r="A60" s="137"/>
-      <c r="B60" s="138"/>
+      <c r="A60" s="135"/>
+      <c r="B60" s="136"/>
       <c r="C60" s="104" t="s">
         <v>49</v>
       </c>
@@ -4178,8 +4348,8 @@
       <c r="AA60" s="92"/>
     </row>
     <row r="61" spans="1:27" ht="15" customHeight="1">
-      <c r="A61" s="137"/>
-      <c r="B61" s="138"/>
+      <c r="A61" s="135"/>
+      <c r="B61" s="136"/>
       <c r="C61" s="104" t="s">
         <v>54</v>
       </c>
@@ -4211,8 +4381,8 @@
       <c r="AA61" s="92"/>
     </row>
     <row r="62" spans="1:27" ht="15" customHeight="1">
-      <c r="A62" s="139"/>
-      <c r="B62" s="140"/>
+      <c r="A62" s="137"/>
+      <c r="B62" s="138"/>
       <c r="C62" s="104" t="s">
         <v>12</v>
       </c>
@@ -4244,10 +4414,10 @@
       <c r="AA62" s="92"/>
     </row>
     <row r="63" spans="1:27" ht="15" customHeight="1">
-      <c r="A63" s="141" t="s">
+      <c r="A63" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="142"/>
+      <c r="B63" s="140"/>
       <c r="C63" s="106" t="s">
         <v>8</v>
       </c>
@@ -4279,8 +4449,8 @@
       <c r="AA63" s="108"/>
     </row>
     <row r="64" spans="1:27" ht="15" customHeight="1">
-      <c r="A64" s="143"/>
-      <c r="B64" s="144"/>
+      <c r="A64" s="141"/>
+      <c r="B64" s="142"/>
       <c r="C64" s="106" t="s">
         <v>7</v>
       </c>
@@ -4312,8 +4482,8 @@
       <c r="AA64" s="108"/>
     </row>
     <row r="65" spans="1:27" ht="15" customHeight="1">
-      <c r="A65" s="143"/>
-      <c r="B65" s="144"/>
+      <c r="A65" s="141"/>
+      <c r="B65" s="142"/>
       <c r="C65" s="106" t="s">
         <v>48</v>
       </c>
@@ -4345,8 +4515,8 @@
       <c r="AA65" s="108"/>
     </row>
     <row r="66" spans="1:27" ht="15" customHeight="1">
-      <c r="A66" s="143"/>
-      <c r="B66" s="144"/>
+      <c r="A66" s="141"/>
+      <c r="B66" s="142"/>
       <c r="C66" s="106" t="s">
         <v>49</v>
       </c>
@@ -4378,8 +4548,8 @@
       <c r="AA66" s="108"/>
     </row>
     <row r="67" spans="1:27" ht="15" customHeight="1">
-      <c r="A67" s="143"/>
-      <c r="B67" s="144"/>
+      <c r="A67" s="141"/>
+      <c r="B67" s="142"/>
       <c r="C67" s="106" t="s">
         <v>54</v>
       </c>
@@ -4411,8 +4581,8 @@
       <c r="AA67" s="108"/>
     </row>
     <row r="68" spans="1:27" ht="15" customHeight="1">
-      <c r="A68" s="145"/>
-      <c r="B68" s="146"/>
+      <c r="A68" s="143"/>
+      <c r="B68" s="144"/>
       <c r="C68" s="106" t="s">
         <v>12</v>
       </c>
@@ -4444,10 +4614,10 @@
       <c r="AA68" s="108"/>
     </row>
     <row r="69" spans="1:27" ht="15" customHeight="1">
-      <c r="A69" s="147" t="s">
+      <c r="A69" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="148"/>
+      <c r="B69" s="146"/>
       <c r="C69" s="110" t="s">
         <v>8</v>
       </c>
@@ -4479,8 +4649,8 @@
       <c r="AA69" s="92"/>
     </row>
     <row r="70" spans="1:27" ht="15" customHeight="1">
-      <c r="A70" s="149"/>
-      <c r="B70" s="150"/>
+      <c r="A70" s="147"/>
+      <c r="B70" s="148"/>
       <c r="C70" s="110" t="s">
         <v>54</v>
       </c>
@@ -4512,8 +4682,8 @@
       <c r="AA70" s="92"/>
     </row>
     <row r="71" spans="1:27" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A71" s="151"/>
-      <c r="B71" s="152"/>
+      <c r="A71" s="149"/>
+      <c r="B71" s="150"/>
       <c r="C71" s="112" t="s">
         <v>12</v>
       </c>

</xml_diff>